<commit_message>
Levantamiento del módulo de solicitudes vehículares. Agregados: Incorporación de estados en index de solicitudes.
</commit_message>
<xml_diff>
--- a/storage/excel/Hoja de salida.xlsx
+++ b/storage/excel/Hoja de salida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8b9d410b455542aa/Escritorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1887" documentId="8_{B420F790-D364-4D97-9603-65FD549F4D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EFC15A6-261F-424C-A2F5-7E04D305D122}"/>
+  <xr:revisionPtr revIDLastSave="2204" documentId="8_{B420F790-D364-4D97-9603-65FD549F4D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4229C86-5634-41E8-980C-374E9B0F5D24}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="873" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="873" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud de Vehiculo" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Solicitante!$B$1:$D$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">Hoja2!$N$48:$O$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Solicitante!$B$2:$D$362</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitud de Vehiculo'!$A$1:$I$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitud de Vehiculo'!$B$1:$J$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Solicitud de Vehiculo (2)'!$B$1:$J$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="1652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1658">
   <si>
     <t xml:space="preserve">LUNES </t>
   </si>
@@ -4924,21 +4924,9 @@
     <t>Dirección regional:</t>
   </si>
   <si>
-    <t>Fecha salida de vehículo:</t>
-  </si>
-  <si>
-    <t>Fecha regreso de vehículo:</t>
-  </si>
-  <si>
     <t>DATOS DE OCUPANTES</t>
   </si>
   <si>
-    <t>NroBitácora</t>
-  </si>
-  <si>
-    <t>ABASTECIÓ BENCINA</t>
-  </si>
-  <si>
     <t>FECHA</t>
   </si>
   <si>
@@ -4978,34 +4966,64 @@
     <t>7° Ocupante:</t>
   </si>
   <si>
-    <t>8° Ocupante:</t>
-  </si>
-  <si>
     <t>Jefatura asociada:</t>
   </si>
   <si>
-    <t>Hora salida:</t>
-  </si>
-  <si>
-    <t>Hora regreso:</t>
-  </si>
-  <si>
-    <t>Hora inicio OT:</t>
-  </si>
-  <si>
     <t>N° Orden Trabajo:</t>
   </si>
   <si>
-    <t>Hora inicio conducción:</t>
-  </si>
-  <si>
-    <t>Hora término conducción:</t>
-  </si>
-  <si>
-    <t>Hora término OT:</t>
-  </si>
-  <si>
     <t>Firma jefe que autoriza:</t>
+  </si>
+  <si>
+    <t>Total en horas conducción:</t>
+  </si>
+  <si>
+    <t>Nivel de estanque:</t>
+  </si>
+  <si>
+    <t>Número de bitácora:</t>
+  </si>
+  <si>
+    <t>¿Abasteció bencina?</t>
+  </si>
+  <si>
+    <t>Kilometraje al retornar:</t>
+  </si>
+  <si>
+    <t>Fecha de reingreso:</t>
+  </si>
+  <si>
+    <t>Hora de reingreso:</t>
+  </si>
+  <si>
+    <t>Total kilómetros recorridos:</t>
+  </si>
+  <si>
+    <t>Kilometraje al salir:</t>
+  </si>
+  <si>
+    <t>Hora de salida:</t>
+  </si>
+  <si>
+    <t>Hora de regreso:</t>
+  </si>
+  <si>
+    <t>Hora de inicio Orden Trabajo:</t>
+  </si>
+  <si>
+    <t>Hora de término Orden Trabajo:</t>
+  </si>
+  <si>
+    <t>Hora de inicio conducción:</t>
+  </si>
+  <si>
+    <t>Hora de término conducción:</t>
+  </si>
+  <si>
+    <t>Fecha de salida asignada:</t>
+  </si>
+  <si>
+    <t>Fecha de regreso asignada:</t>
   </si>
 </sst>
 </file>
@@ -5337,12 +5355,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -5395,8 +5407,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7BD00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="79">
+  <borders count="80">
     <border>
       <left/>
       <right/>
@@ -6380,11 +6398,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="326">
+  <cellXfs count="341">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6687,19 +6720,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6767,10 +6800,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -6794,414 +6823,478 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="40" fillId="19" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="40" fillId="19" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="61" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="66" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="20" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="39" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="39" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="18" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="18" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="18" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="40" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="40" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="40" fillId="20" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="40" fillId="20" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="40" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="61" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="66" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="19" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="19" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="19" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7445,6 +7538,7 @@
   <colors>
     <mruColors>
       <color rgb="FFDDEBF7"/>
+      <color rgb="FFF7BD00"/>
       <color rgb="FFE6500A"/>
       <color rgb="FFFF6600"/>
       <color rgb="FF9CCFEE"/>
@@ -7471,126 +7565,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:colOff>122727</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>136423</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>236220</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32400" name="Line 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000907E0000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1920240" y="9563100"/>
-          <a:ext cx="3642360" cy="7620"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="sysDot"/>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>360861</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>367393</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>862148</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>39733</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32401" name="Rectangle 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000917E0000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4905647" y="9674679"/>
-          <a:ext cx="501287" cy="434340"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>3922</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>750794</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>3922</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552827</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>136423</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7607,8 +7590,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="3720353" y="16005922"/>
-          <a:ext cx="12147176" cy="0"/>
+          <a:off x="959068" y="7198862"/>
+          <a:ext cx="4793015" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7636,15 +7619,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7690,15 +7673,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7742,430 +7725,16 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>329837</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>250372</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>215537</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32406" name="Rectangle 53">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000967E0000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5139146" y="9256123"/>
-          <a:ext cx="1248047" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>678180</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32407" name="Rectangle 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000977E0000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3665220" y="9715500"/>
-          <a:ext cx="1158240" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>868680</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32408" name="Rectangle 55">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000987E0000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6736080" y="9738360"/>
-          <a:ext cx="807720" cy="289560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>205740</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32409" name="Oval 57">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000997E0000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3665220" y="10020300"/>
-          <a:ext cx="762000" cy="548640"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>49877</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>868681</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>327660</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 55">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6724997" y="10157460"/>
-          <a:ext cx="818804" cy="327660"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>49877</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>64424</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>320040</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectangle 55">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6724997" y="9398924"/>
-          <a:ext cx="384463" cy="255616"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-CL"/>
-            <a:t>SI</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>491837</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>64424</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>320040</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectangle 55">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7166957" y="9398924"/>
-          <a:ext cx="384463" cy="255616"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="22225">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CL"/>
-            <a:t>NO</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>73269</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>86904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>369980</xdr:colOff>
+      <xdr:colOff>293617</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>4884</xdr:rowOff>
     </xdr:to>
@@ -8202,7 +7771,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
@@ -9083,10 +8652,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -9435,598 +9000,588 @@
     <tabColor theme="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V36"/>
+  <dimension ref="B1:W35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="131" customWidth="1"/>
-    <col min="2" max="2" width="3" style="131" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="131" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="131" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="131" customWidth="1"/>
-    <col min="6" max="6" width="13" style="131" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="131" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="131" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="131" customWidth="1"/>
-    <col min="10" max="10" width="3.140625" style="131" customWidth="1"/>
-    <col min="11" max="14" width="11.42578125" style="131" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="131"/>
+    <col min="1" max="1" width="3.28515625" style="131" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="131" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="131" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="131" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="131" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="131" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="131" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="131" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="131" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" style="131" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="131" customWidth="1"/>
+    <col min="12" max="15" width="11.42578125" style="131" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="131"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15">
-      <c r="A1" s="140"/>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="241"/>
-      <c r="E1" s="241"/>
-      <c r="F1" s="241"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="142"/>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="204" t="s">
-        <v>1629</v>
-      </c>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="143" t="s">
-        <v>1630</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="15">
-      <c r="A3" s="139"/>
-      <c r="B3" s="156"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="247" t="s">
+    <row r="1" spans="2:23" ht="15">
+      <c r="B1" s="139"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="253"/>
+      <c r="F1" s="253"/>
+      <c r="G1" s="253"/>
+      <c r="H1" s="252"/>
+      <c r="I1" s="252"/>
+      <c r="J1" s="141"/>
+    </row>
+    <row r="2" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B2" s="136"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="262" t="s">
+        <v>1625</v>
+      </c>
+      <c r="F2" s="262"/>
+      <c r="G2" s="262"/>
+      <c r="H2" s="262"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="142" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" ht="15">
+      <c r="B3" s="138"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="259" t="s">
         <v>1614</v>
       </c>
-      <c r="E3" s="248"/>
-      <c r="F3" s="153" t="s">
+      <c r="F3" s="260"/>
+      <c r="G3" s="143" t="s">
         <v>1615</v>
       </c>
-      <c r="G3" s="153" t="s">
+      <c r="H3" s="143" t="s">
         <v>1616</v>
       </c>
-      <c r="H3" s="155"/>
-      <c r="I3" s="245"/>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A4" s="137"/>
-      <c r="B4" s="155"/>
-      <c r="C4" s="157"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="246"/>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A5" s="137"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="155"/>
-      <c r="H5" s="158" t="s">
+      <c r="I3" s="177"/>
+      <c r="J3" s="257"/>
+    </row>
+    <row r="4" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B4" s="136"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="179"/>
+      <c r="E4" s="196"/>
+      <c r="F4" s="196"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="196"/>
+      <c r="I4" s="177"/>
+      <c r="J4" s="258"/>
+    </row>
+    <row r="5" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B5" s="136"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="177"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="138"/>
-    </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A6" s="242" t="s">
+      <c r="J5" s="137"/>
+    </row>
+    <row r="6" spans="2:23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B6" s="254" t="s">
         <v>1613</v>
       </c>
-      <c r="B6" s="243"/>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="243"/>
-      <c r="I6" s="244"/>
-    </row>
-    <row r="7" spans="1:22" ht="16.5">
-      <c r="A7" s="189" t="s">
+      <c r="C6" s="255"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
+      <c r="H6" s="255"/>
+      <c r="I6" s="255"/>
+      <c r="J6" s="256"/>
+    </row>
+    <row r="7" spans="2:23" ht="15">
+      <c r="B7" s="161" t="s">
         <v>1617</v>
       </c>
-      <c r="B7" s="208"/>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="183" t="s">
+      <c r="C7" s="245"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="155" t="s">
         <v>1620</v>
       </c>
-      <c r="G7" s="205"/>
-      <c r="H7" s="206"/>
-      <c r="I7" s="207"/>
-    </row>
-    <row r="8" spans="1:22" ht="16.5" thickBot="1">
-      <c r="A8" s="190" t="s">
+      <c r="H7" s="242"/>
+      <c r="I7" s="243"/>
+      <c r="J7" s="244"/>
+    </row>
+    <row r="8" spans="2:23" ht="16.5" thickBot="1">
+      <c r="B8" s="162" t="s">
         <v>1623</v>
       </c>
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="213"/>
-      <c r="F8" s="184" t="s">
+      <c r="C8" s="250"/>
+      <c r="D8" s="251"/>
+      <c r="E8" s="251"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="156" t="s">
         <v>1619</v>
       </c>
-      <c r="G8" s="210"/>
-      <c r="H8" s="211"/>
-      <c r="I8" s="212"/>
-      <c r="J8" s="133"/>
+      <c r="H8" s="247"/>
+      <c r="I8" s="248"/>
+      <c r="J8" s="249"/>
       <c r="K8" s="133"/>
       <c r="L8" s="133"/>
       <c r="M8" s="133"/>
       <c r="N8" s="133"/>
-    </row>
-    <row r="9" spans="1:22" ht="15">
-      <c r="A9" s="191" t="s">
+      <c r="O8" s="133"/>
+    </row>
+    <row r="9" spans="2:23" ht="15">
+      <c r="B9" s="163" t="s">
         <v>1618</v>
       </c>
-      <c r="B9" s="201"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="185" t="s">
-        <v>1647</v>
-      </c>
-      <c r="G9" s="168"/>
-      <c r="H9" s="194" t="s">
-        <v>1646</v>
-      </c>
-      <c r="I9" s="172"/>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A10" s="190" t="s">
+      <c r="C9" s="206"/>
+      <c r="D9" s="207"/>
+      <c r="E9" s="207"/>
+      <c r="F9" s="207"/>
+      <c r="G9" s="157" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H9" s="146"/>
+      <c r="I9" s="166" t="s">
+        <v>1652</v>
+      </c>
+      <c r="J9" s="148"/>
+    </row>
+    <row r="10" spans="2:23" ht="17.25" thickBot="1">
+      <c r="B10" s="162" t="s">
         <v>1622</v>
       </c>
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="186" t="s">
+      <c r="C10" s="217"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="158" t="s">
         <v>1621</v>
       </c>
-      <c r="G10" s="169"/>
-      <c r="H10" s="195" t="s">
+      <c r="H10" s="147"/>
+      <c r="I10" s="167" t="s">
+        <v>1653</v>
+      </c>
+      <c r="J10" s="149"/>
+    </row>
+    <row r="11" spans="2:23" ht="15">
+      <c r="B11" s="164" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C11" s="192"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="193"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="159" t="s">
         <v>1650</v>
       </c>
-      <c r="I10" s="173"/>
-    </row>
-    <row r="11" spans="1:22" ht="16.5">
-      <c r="A11" s="192" t="s">
+      <c r="H11" s="198"/>
+      <c r="I11" s="168" t="s">
+        <v>1654</v>
+      </c>
+      <c r="J11" s="150"/>
+    </row>
+    <row r="12" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B12" s="165" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C12" s="194"/>
+      <c r="D12" s="195"/>
+      <c r="E12" s="195"/>
+      <c r="F12" s="195"/>
+      <c r="G12" s="160" t="s">
+        <v>1651</v>
+      </c>
+      <c r="H12" s="199"/>
+      <c r="I12" s="169" t="s">
+        <v>1655</v>
+      </c>
+      <c r="J12" s="151"/>
+    </row>
+    <row r="13" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B13" s="210" t="s">
         <v>1624</v>
       </c>
-      <c r="B11" s="176"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="177"/>
-      <c r="E11" s="177"/>
-      <c r="F11" s="187" t="s">
-        <v>1644</v>
-      </c>
-      <c r="G11" s="170"/>
-      <c r="H11" s="196" t="s">
-        <v>1648</v>
-      </c>
-      <c r="I11" s="174"/>
-    </row>
-    <row r="12" spans="1:22" ht="17.25" thickBot="1">
-      <c r="A12" s="193" t="s">
-        <v>1625</v>
-      </c>
-      <c r="B12" s="178"/>
-      <c r="C12" s="179"/>
-      <c r="D12" s="179"/>
-      <c r="E12" s="179"/>
-      <c r="F12" s="188" t="s">
-        <v>1645</v>
-      </c>
-      <c r="G12" s="171"/>
-      <c r="H12" s="197" t="s">
-        <v>1649</v>
-      </c>
-      <c r="I12" s="175"/>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A13" s="218" t="s">
-        <v>1626</v>
-      </c>
-      <c r="B13" s="219"/>
-      <c r="C13" s="219"/>
-      <c r="D13" s="219"/>
-      <c r="E13" s="228"/>
-      <c r="F13" s="228"/>
-      <c r="G13" s="219"/>
-      <c r="H13" s="219"/>
-      <c r="I13" s="220"/>
-      <c r="P13" s="132"/>
+      <c r="C13" s="211"/>
+      <c r="D13" s="211"/>
+      <c r="E13" s="211"/>
+      <c r="F13" s="261"/>
+      <c r="G13" s="261"/>
+      <c r="H13" s="211"/>
+      <c r="I13" s="211"/>
+      <c r="J13" s="212"/>
       <c r="Q13" s="132"/>
       <c r="R13" s="132"/>
       <c r="S13" s="132"/>
       <c r="T13" s="132"/>
       <c r="U13" s="132"/>
       <c r="V13" s="132"/>
-    </row>
-    <row r="14" spans="1:22" ht="15">
-      <c r="A14" s="199" t="s">
+      <c r="W13" s="132"/>
+    </row>
+    <row r="14" spans="2:23" ht="15">
+      <c r="B14" s="171" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C14" s="235"/>
+      <c r="D14" s="236"/>
+      <c r="E14" s="236"/>
+      <c r="F14" s="216"/>
+      <c r="G14" s="155" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H14" s="235"/>
+      <c r="I14" s="236"/>
+      <c r="J14" s="263"/>
+    </row>
+    <row r="15" spans="2:23" ht="15">
+      <c r="B15" s="163" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C15" s="206"/>
+      <c r="D15" s="207"/>
+      <c r="E15" s="207"/>
+      <c r="F15" s="209"/>
+      <c r="G15" s="170" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H15" s="206"/>
+      <c r="I15" s="207"/>
+      <c r="J15" s="208"/>
+    </row>
+    <row r="16" spans="2:23" ht="15">
+      <c r="B16" s="163" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C16" s="206"/>
+      <c r="D16" s="207"/>
+      <c r="E16" s="207"/>
+      <c r="F16" s="209"/>
+      <c r="G16" s="170" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H16" s="206"/>
+      <c r="I16" s="207"/>
+      <c r="J16" s="208"/>
+    </row>
+    <row r="17" spans="2:10" ht="15">
+      <c r="B17" s="163" t="s">
+        <v>1634</v>
+      </c>
+      <c r="C17" s="206"/>
+      <c r="D17" s="207"/>
+      <c r="E17" s="207"/>
+      <c r="F17" s="209"/>
+      <c r="G17" s="170" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H17" s="206"/>
+      <c r="I17" s="207"/>
+      <c r="J17" s="208"/>
+    </row>
+    <row r="18" spans="2:10" ht="15">
+      <c r="B18" s="163" t="s">
         <v>1635</v>
       </c>
-      <c r="B14" s="205"/>
-      <c r="C14" s="206"/>
-      <c r="D14" s="206"/>
-      <c r="E14" s="223"/>
-      <c r="F14" s="183" t="s">
+      <c r="C18" s="206"/>
+      <c r="D18" s="207"/>
+      <c r="E18" s="207"/>
+      <c r="F18" s="209"/>
+      <c r="G18" s="170" t="s">
         <v>1618</v>
       </c>
-      <c r="G14" s="205"/>
-      <c r="H14" s="206"/>
-      <c r="I14" s="207"/>
-    </row>
-    <row r="15" spans="1:22" ht="15">
-      <c r="A15" s="191" t="s">
+      <c r="H18" s="206"/>
+      <c r="I18" s="207"/>
+      <c r="J18" s="208"/>
+    </row>
+    <row r="19" spans="2:10" ht="15">
+      <c r="B19" s="163" t="s">
         <v>1636</v>
       </c>
-      <c r="B15" s="201"/>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="217"/>
-      <c r="F15" s="198" t="s">
+      <c r="C19" s="206"/>
+      <c r="D19" s="207"/>
+      <c r="E19" s="207"/>
+      <c r="F19" s="209"/>
+      <c r="G19" s="170" t="s">
         <v>1618</v>
       </c>
-      <c r="G15" s="201"/>
-      <c r="H15" s="202"/>
-      <c r="I15" s="203"/>
-    </row>
-    <row r="16" spans="1:22" ht="15">
-      <c r="A16" s="191" t="s">
+      <c r="H19" s="206"/>
+      <c r="I19" s="207"/>
+      <c r="J19" s="208"/>
+    </row>
+    <row r="20" spans="2:10" ht="15">
+      <c r="B20" s="163" t="s">
         <v>1637</v>
       </c>
-      <c r="B16" s="201"/>
-      <c r="C16" s="202"/>
-      <c r="D16" s="202"/>
-      <c r="E16" s="217"/>
-      <c r="F16" s="198" t="s">
+      <c r="C20" s="206"/>
+      <c r="D20" s="207"/>
+      <c r="E20" s="207"/>
+      <c r="F20" s="209"/>
+      <c r="G20" s="170" t="s">
         <v>1618</v>
       </c>
-      <c r="G16" s="201"/>
-      <c r="H16" s="202"/>
-      <c r="I16" s="203"/>
-    </row>
-    <row r="17" spans="1:9" ht="15">
-      <c r="A17" s="191" t="s">
+      <c r="H20" s="206"/>
+      <c r="I20" s="207"/>
+      <c r="J20" s="208"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B21" s="134"/>
+      <c r="C21" s="181"/>
+      <c r="D21" s="224"/>
+      <c r="E21" s="224"/>
+      <c r="F21" s="276"/>
+      <c r="G21" s="276"/>
+      <c r="H21" s="276"/>
+      <c r="I21" s="276"/>
+      <c r="J21" s="135"/>
+    </row>
+    <row r="22" spans="2:10" ht="15">
+      <c r="B22" s="277" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C22" s="278"/>
+      <c r="D22" s="265"/>
+      <c r="E22" s="266"/>
+      <c r="F22" s="267"/>
+      <c r="G22" s="274" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H22" s="271"/>
+      <c r="I22" s="272"/>
+      <c r="J22" s="273"/>
+    </row>
+    <row r="23" spans="2:10" ht="13.5" customHeight="1">
+      <c r="B23" s="215"/>
+      <c r="C23" s="216"/>
+      <c r="D23" s="268"/>
+      <c r="E23" s="269"/>
+      <c r="F23" s="270"/>
+      <c r="G23" s="275"/>
+      <c r="H23" s="235"/>
+      <c r="I23" s="236"/>
+      <c r="J23" s="263"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B24" s="264"/>
+      <c r="C24" s="218"/>
+      <c r="D24" s="218"/>
+      <c r="E24" s="218"/>
+      <c r="F24" s="219"/>
+      <c r="G24" s="172" t="s">
         <v>1638</v>
       </c>
-      <c r="B17" s="201"/>
-      <c r="C17" s="202"/>
-      <c r="D17" s="202"/>
-      <c r="E17" s="217"/>
-      <c r="F17" s="198" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G17" s="201"/>
-      <c r="H17" s="202"/>
-      <c r="I17" s="203"/>
-    </row>
-    <row r="18" spans="1:9" ht="15">
-      <c r="A18" s="191" t="s">
-        <v>1639</v>
-      </c>
-      <c r="B18" s="201"/>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="217"/>
-      <c r="F18" s="198" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G18" s="201"/>
-      <c r="H18" s="202"/>
-      <c r="I18" s="203"/>
-    </row>
-    <row r="19" spans="1:9" ht="15">
-      <c r="A19" s="191" t="s">
-        <v>1640</v>
-      </c>
-      <c r="B19" s="201"/>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="217"/>
-      <c r="F19" s="198" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G19" s="201"/>
-      <c r="H19" s="202"/>
-      <c r="I19" s="203"/>
-    </row>
-    <row r="20" spans="1:9" ht="15">
-      <c r="A20" s="191" t="s">
+      <c r="H24" s="217"/>
+      <c r="I24" s="218"/>
+      <c r="J24" s="219"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B25" s="134"/>
+      <c r="C25" s="181"/>
+      <c r="D25" s="181"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="181"/>
+      <c r="G25" s="182"/>
+      <c r="H25" s="181"/>
+      <c r="I25" s="181"/>
+      <c r="J25" s="135"/>
+    </row>
+    <row r="26" spans="2:10" ht="16.5" customHeight="1">
+      <c r="B26" s="134"/>
+      <c r="C26" s="181"/>
+      <c r="D26" s="181"/>
+      <c r="E26" s="181"/>
+      <c r="F26" s="183"/>
+      <c r="G26" s="228" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H26" s="229"/>
+      <c r="I26" s="229"/>
+      <c r="J26" s="230"/>
+    </row>
+    <row r="27" spans="2:10" ht="15">
+      <c r="B27" s="213" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C27" s="214"/>
+      <c r="D27" s="220"/>
+      <c r="E27" s="221"/>
+      <c r="F27" s="221"/>
+      <c r="G27" s="145" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="144"/>
+      <c r="I27" s="231" t="s">
+        <v>1630</v>
+      </c>
+      <c r="J27" s="232"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B28" s="215"/>
+      <c r="C28" s="216"/>
+      <c r="D28" s="222"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="153"/>
+      <c r="H28" s="154"/>
+      <c r="I28" s="233"/>
+      <c r="J28" s="234"/>
+    </row>
+    <row r="29" spans="2:10" ht="24.75" customHeight="1" thickBot="1">
+      <c r="B29" s="225" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="226"/>
+      <c r="D29" s="226"/>
+      <c r="E29" s="226"/>
+      <c r="F29" s="226"/>
+      <c r="G29" s="226"/>
+      <c r="H29" s="226"/>
+      <c r="I29" s="226"/>
+      <c r="J29" s="227"/>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B30" s="210" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="211"/>
+      <c r="D30" s="211"/>
+      <c r="E30" s="211"/>
+      <c r="F30" s="211"/>
+      <c r="G30" s="211"/>
+      <c r="H30" s="211"/>
+      <c r="I30" s="211"/>
+      <c r="J30" s="212"/>
+    </row>
+    <row r="31" spans="2:10" ht="15">
+      <c r="B31" s="173" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C31" s="152"/>
+      <c r="D31" s="152"/>
+      <c r="E31" s="152"/>
+      <c r="F31" s="152"/>
+      <c r="G31" s="175" t="s">
+        <v>1649</v>
+      </c>
+      <c r="H31" s="188"/>
+      <c r="I31" s="189" t="s">
+        <v>1643</v>
+      </c>
+      <c r="J31" s="185"/>
+    </row>
+    <row r="32" spans="2:10" ht="15">
+      <c r="B32" s="174" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C32" s="237"/>
+      <c r="D32" s="238"/>
+      <c r="E32" s="238"/>
+      <c r="F32" s="239"/>
+      <c r="G32" s="176" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H32" s="184"/>
+      <c r="I32" s="190" t="s">
+        <v>1644</v>
+      </c>
+      <c r="J32" s="186"/>
+    </row>
+    <row r="33" spans="2:10" ht="16.5">
+      <c r="B33" s="158" t="s">
         <v>1641</v>
       </c>
-      <c r="B20" s="201"/>
-      <c r="C20" s="202"/>
-      <c r="D20" s="202"/>
-      <c r="E20" s="217"/>
-      <c r="F20" s="198" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G20" s="201"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="203"/>
-    </row>
-    <row r="21" spans="1:9" ht="15">
-      <c r="A21" s="191" t="s">
+      <c r="C33" s="240"/>
+      <c r="D33" s="240"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="241"/>
+      <c r="G33" s="169" t="s">
+        <v>1648</v>
+      </c>
+      <c r="H33" s="191"/>
+      <c r="I33" s="170" t="s">
         <v>1642</v>
       </c>
-      <c r="B21" s="201"/>
-      <c r="C21" s="202"/>
-      <c r="D21" s="202"/>
-      <c r="E21" s="217"/>
-      <c r="F21" s="198" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G21" s="201"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="203"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A22" s="134"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="229"/>
-      <c r="D22" s="229"/>
-      <c r="E22" s="261"/>
-      <c r="F22" s="261"/>
-      <c r="G22" s="261"/>
-      <c r="H22" s="261"/>
-      <c r="I22" s="135"/>
-    </row>
-    <row r="23" spans="1:9" ht="15">
-      <c r="A23" s="262" t="s">
-        <v>1632</v>
-      </c>
-      <c r="B23" s="263"/>
-      <c r="C23" s="250"/>
-      <c r="D23" s="251"/>
-      <c r="E23" s="252"/>
-      <c r="F23" s="259" t="s">
-        <v>1651</v>
-      </c>
-      <c r="G23" s="256"/>
-      <c r="H23" s="257"/>
-      <c r="I23" s="258"/>
-    </row>
-    <row r="24" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A24" s="222"/>
-      <c r="B24" s="223"/>
-      <c r="C24" s="253"/>
-      <c r="D24" s="254"/>
-      <c r="E24" s="255"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="205"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="207"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A25" s="249"/>
-      <c r="B25" s="215"/>
-      <c r="C25" s="215"/>
-      <c r="D25" s="215"/>
-      <c r="E25" s="216"/>
-      <c r="F25" s="200" t="s">
-        <v>1643</v>
-      </c>
-      <c r="G25" s="214"/>
-      <c r="H25" s="215"/>
-      <c r="I25" s="216"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A26" s="134"/>
-      <c r="B26" s="151"/>
-      <c r="C26" s="151"/>
-      <c r="D26" s="151"/>
-      <c r="E26" s="151"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="151"/>
-      <c r="H26" s="151"/>
-      <c r="I26" s="135"/>
-    </row>
-    <row r="27" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A27" s="134"/>
-      <c r="B27" s="151"/>
-      <c r="C27" s="151"/>
-      <c r="D27" s="151"/>
-      <c r="E27" s="160"/>
-      <c r="F27" s="233" t="s">
-        <v>1633</v>
-      </c>
-      <c r="G27" s="234"/>
-      <c r="H27" s="234"/>
-      <c r="I27" s="235"/>
-    </row>
-    <row r="28" spans="1:9" ht="15">
-      <c r="A28" s="221" t="s">
-        <v>1631</v>
-      </c>
-      <c r="B28" s="213"/>
-      <c r="C28" s="224"/>
-      <c r="D28" s="225"/>
-      <c r="E28" s="225"/>
-      <c r="F28" s="167" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="154"/>
-      <c r="H28" s="236" t="s">
-        <v>1634</v>
-      </c>
-      <c r="I28" s="237"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A29" s="222"/>
-      <c r="B29" s="223"/>
-      <c r="C29" s="226"/>
-      <c r="D29" s="227"/>
-      <c r="E29" s="227"/>
-      <c r="F29" s="181"/>
-      <c r="G29" s="182"/>
-      <c r="H29" s="238"/>
-      <c r="I29" s="239"/>
-    </row>
-    <row r="30" spans="1:9" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A30" s="230" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="231"/>
-      <c r="C30" s="231"/>
-      <c r="D30" s="231"/>
-      <c r="E30" s="231"/>
-      <c r="F30" s="231"/>
-      <c r="G30" s="231"/>
-      <c r="H30" s="231"/>
-      <c r="I30" s="232"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A31" s="218" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="219"/>
-      <c r="C31" s="219"/>
-      <c r="D31" s="219"/>
-      <c r="E31" s="219"/>
-      <c r="F31" s="219"/>
-      <c r="G31" s="219"/>
-      <c r="H31" s="219"/>
-      <c r="I31" s="220"/>
-    </row>
-    <row r="32" spans="1:9" ht="24.75">
-      <c r="A32" s="136" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="161"/>
-      <c r="C32" s="151"/>
-      <c r="D32" s="151"/>
-      <c r="E32" s="151"/>
-      <c r="F32" s="151"/>
-      <c r="G32" s="160" t="s">
-        <v>1628</v>
-      </c>
-      <c r="H32" s="157"/>
-      <c r="I32" s="135"/>
-    </row>
-    <row r="33" spans="1:9" ht="24.75">
-      <c r="A33" s="144" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="162"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="163" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="151"/>
-      <c r="F33" s="151"/>
-      <c r="G33" s="160" t="s">
-        <v>48</v>
-      </c>
-      <c r="H33" s="151"/>
-      <c r="I33" s="135"/>
-    </row>
-    <row r="34" spans="1:9" ht="15">
-      <c r="A34" s="144"/>
-      <c r="B34" s="162"/>
-      <c r="C34" s="152"/>
-      <c r="D34" s="163"/>
-      <c r="E34" s="151"/>
-      <c r="F34" s="151"/>
-      <c r="G34" s="164"/>
-      <c r="H34" s="151"/>
-      <c r="I34" s="135"/>
-    </row>
-    <row r="35" spans="1:9" ht="16.5">
-      <c r="A35" s="145" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="165"/>
-      <c r="C35" s="165"/>
-      <c r="D35" s="161" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="151"/>
-      <c r="F35" s="151"/>
-      <c r="G35" s="166" t="s">
-        <v>1627</v>
-      </c>
-      <c r="H35" s="151"/>
-      <c r="I35" s="135"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A36" s="146" t="s">
+      <c r="J33" s="187"/>
+    </row>
+    <row r="34" spans="2:10" ht="15">
+      <c r="B34" s="200" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="147"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="148"/>
-      <c r="F36" s="148"/>
-      <c r="G36" s="149"/>
-      <c r="H36" s="148"/>
-      <c r="I36" s="150"/>
+      <c r="C34" s="202"/>
+      <c r="D34" s="202"/>
+      <c r="E34" s="202"/>
+      <c r="F34" s="202"/>
+      <c r="G34" s="202"/>
+      <c r="H34" s="202"/>
+      <c r="I34" s="202"/>
+      <c r="J34" s="203"/>
+    </row>
+    <row r="35" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B35" s="201"/>
+      <c r="C35" s="204"/>
+      <c r="D35" s="204"/>
+      <c r="E35" s="204"/>
+      <c r="F35" s="204"/>
+      <c r="G35" s="204"/>
+      <c r="H35" s="204"/>
+      <c r="I35" s="204"/>
+      <c r="J35" s="205"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="C23:E24"/>
-    <mergeCell ref="G23:I24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="A23:B24"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="C28:E29"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
+  <mergeCells count="46">
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="D22:F23"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:J35"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="D27:F28"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H22:J23"/>
+    <mergeCell ref="G22:G23"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -10041,24 +9596,24 @@
   </webPublishItems>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Hoja2!$O$47:$O$64</xm:f>
           </x14:formula1>
-          <xm:sqref>F29 H29</xm:sqref>
+          <xm:sqref>G28 I28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Hoja3!$I$1:$I$55</xm:f>
           </x14:formula1>
-          <xm:sqref>A25:B25</xm:sqref>
+          <xm:sqref>B24:C24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Hoja2!$C$1:$C$13</xm:f>
           </x14:formula1>
-          <xm:sqref>G4</xm:sqref>
+          <xm:sqref>H4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10099,11 +9654,11 @@
       <c r="B1" s="34"/>
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>
-      <c r="E1" s="306"/>
-      <c r="F1" s="306"/>
-      <c r="G1" s="306"/>
-      <c r="H1" s="307"/>
-      <c r="I1" s="307"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="322"/>
+      <c r="I1" s="322"/>
       <c r="J1" s="55"/>
     </row>
     <row r="2" spans="2:10" ht="13.7" customHeight="1">
@@ -10151,35 +9706,35 @@
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:10" ht="30" customHeight="1" thickBot="1">
-      <c r="B6" s="308" t="s">
+      <c r="B6" s="323" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="309"/>
-      <c r="D6" s="309"/>
-      <c r="E6" s="309"/>
-      <c r="F6" s="309"/>
-      <c r="G6" s="309"/>
-      <c r="H6" s="309"/>
-      <c r="I6" s="310"/>
+      <c r="C6" s="324"/>
+      <c r="D6" s="324"/>
+      <c r="E6" s="324"/>
+      <c r="F6" s="324"/>
+      <c r="G6" s="324"/>
+      <c r="H6" s="324"/>
+      <c r="I6" s="325"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="29.45" customHeight="1" thickBot="1">
       <c r="B7" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="311" t="s">
+      <c r="C7" s="326" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="312"/>
-      <c r="E7" s="313"/>
+      <c r="D7" s="327"/>
+      <c r="E7" s="328"/>
       <c r="F7" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="311" t="s">
+      <c r="G7" s="326" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="312"/>
-      <c r="I7" s="313"/>
+      <c r="H7" s="327"/>
+      <c r="I7" s="328"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" ht="3.6" customHeight="1" thickBot="1">
@@ -10197,11 +9752,11 @@
       <c r="B9" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="296" t="s">
+      <c r="C9" s="311" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="297"/>
-      <c r="E9" s="298"/>
+      <c r="D9" s="312"/>
+      <c r="E9" s="313"/>
       <c r="F9" s="64"/>
       <c r="J9" s="5"/>
     </row>
@@ -10213,31 +9768,31 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10" ht="21.6" customHeight="1" thickBot="1">
-      <c r="B11" s="314" t="s">
+      <c r="B11" s="329" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="315"/>
-      <c r="D11" s="316" t="s">
+      <c r="C11" s="330"/>
+      <c r="D11" s="331" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="316"/>
-      <c r="F11" s="316"/>
-      <c r="G11" s="317"/>
-      <c r="H11" s="318"/>
+      <c r="E11" s="331"/>
+      <c r="F11" s="331"/>
+      <c r="G11" s="332"/>
+      <c r="H11" s="333"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10" ht="20.45" customHeight="1" thickBot="1">
-      <c r="B12" s="319" t="s">
+      <c r="B12" s="334" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="320"/>
-      <c r="D12" s="321" t="s">
+      <c r="C12" s="335"/>
+      <c r="D12" s="336" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="321"/>
-      <c r="F12" s="321"/>
-      <c r="G12" s="322"/>
-      <c r="H12" s="323"/>
+      <c r="E12" s="336"/>
+      <c r="F12" s="336"/>
+      <c r="G12" s="337"/>
+      <c r="H12" s="338"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
@@ -10338,16 +9893,16 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10" ht="17.45" customHeight="1">
-      <c r="B18" s="324" t="s">
+      <c r="B18" s="339" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="325"/>
-      <c r="D18" s="325"/>
-      <c r="E18" s="325"/>
-      <c r="F18" s="325"/>
-      <c r="G18" s="325"/>
-      <c r="H18" s="325"/>
-      <c r="I18" s="325"/>
+      <c r="C18" s="340"/>
+      <c r="D18" s="340"/>
+      <c r="E18" s="340"/>
+      <c r="F18" s="340"/>
+      <c r="G18" s="340"/>
+      <c r="H18" s="340"/>
+      <c r="I18" s="340"/>
       <c r="J18" s="68"/>
     </row>
     <row r="19" spans="2:10" ht="10.9" customHeight="1">
@@ -10359,86 +9914,86 @@
       <c r="B20" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="304" t="s">
+      <c r="C20" s="319" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="304"/>
-      <c r="E20" s="304"/>
-      <c r="F20" s="305"/>
-      <c r="G20" s="305"/>
-      <c r="H20" s="305"/>
-      <c r="I20" s="305"/>
+      <c r="D20" s="319"/>
+      <c r="E20" s="319"/>
+      <c r="F20" s="320"/>
+      <c r="G20" s="320"/>
+      <c r="H20" s="320"/>
+      <c r="I20" s="320"/>
       <c r="J20" s="73"/>
     </row>
     <row r="21" spans="2:10" ht="28.15" customHeight="1">
       <c r="B21" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="304" t="s">
+      <c r="C21" s="319" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="304"/>
-      <c r="E21" s="304"/>
-      <c r="F21" s="305"/>
-      <c r="G21" s="305"/>
-      <c r="H21" s="305"/>
-      <c r="I21" s="305"/>
+      <c r="D21" s="319"/>
+      <c r="E21" s="319"/>
+      <c r="F21" s="320"/>
+      <c r="G21" s="320"/>
+      <c r="H21" s="320"/>
+      <c r="I21" s="320"/>
       <c r="J21" s="73"/>
     </row>
     <row r="22" spans="2:10" ht="28.15" customHeight="1">
       <c r="B22" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="304" t="s">
+      <c r="C22" s="319" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="304"/>
-      <c r="E22" s="304"/>
-      <c r="F22" s="305"/>
-      <c r="G22" s="305"/>
-      <c r="H22" s="305"/>
-      <c r="I22" s="305"/>
+      <c r="D22" s="319"/>
+      <c r="E22" s="319"/>
+      <c r="F22" s="320"/>
+      <c r="G22" s="320"/>
+      <c r="H22" s="320"/>
+      <c r="I22" s="320"/>
       <c r="J22" s="73"/>
     </row>
     <row r="23" spans="2:10" ht="28.15" customHeight="1">
       <c r="B23" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="304" t="s">
+      <c r="C23" s="319" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="304"/>
-      <c r="E23" s="304"/>
-      <c r="F23" s="305"/>
-      <c r="G23" s="305"/>
-      <c r="H23" s="305"/>
-      <c r="I23" s="305"/>
+      <c r="D23" s="319"/>
+      <c r="E23" s="319"/>
+      <c r="F23" s="320"/>
+      <c r="G23" s="320"/>
+      <c r="H23" s="320"/>
+      <c r="I23" s="320"/>
       <c r="J23" s="73"/>
     </row>
     <row r="24" spans="2:10" ht="28.15" customHeight="1">
       <c r="B24" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="287" t="s">
+      <c r="C24" s="302" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="287"/>
-      <c r="E24" s="287"/>
-      <c r="F24" s="288"/>
-      <c r="G24" s="288"/>
-      <c r="H24" s="288"/>
-      <c r="I24" s="288"/>
+      <c r="D24" s="302"/>
+      <c r="E24" s="302"/>
+      <c r="F24" s="303"/>
+      <c r="G24" s="303"/>
+      <c r="H24" s="303"/>
+      <c r="I24" s="303"/>
       <c r="J24" s="74"/>
     </row>
     <row r="25" spans="2:10" ht="28.15" customHeight="1">
       <c r="B25" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="287" t="s">
+      <c r="C25" s="302" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="287"/>
-      <c r="E25" s="287"/>
+      <c r="D25" s="302"/>
+      <c r="E25" s="302"/>
       <c r="F25" s="125"/>
       <c r="G25" s="125"/>
       <c r="H25" s="125"/>
@@ -10447,13 +10002,13 @@
     </row>
     <row r="26" spans="2:10" ht="28.15" customHeight="1">
       <c r="B26" s="129"/>
-      <c r="C26" s="289"/>
-      <c r="D26" s="289"/>
-      <c r="E26" s="289"/>
-      <c r="F26" s="290"/>
-      <c r="G26" s="290"/>
-      <c r="H26" s="290"/>
-      <c r="I26" s="290"/>
+      <c r="C26" s="304"/>
+      <c r="D26" s="304"/>
+      <c r="E26" s="304"/>
+      <c r="F26" s="305"/>
+      <c r="G26" s="305"/>
+      <c r="H26" s="305"/>
+      <c r="I26" s="305"/>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="2:10" ht="15.6" customHeight="1">
@@ -10462,13 +10017,13 @@
     </row>
     <row r="28" spans="2:10" ht="9.6" customHeight="1">
       <c r="B28" s="4"/>
-      <c r="C28" s="291"/>
-      <c r="D28" s="291"/>
-      <c r="E28" s="291"/>
-      <c r="F28" s="292"/>
-      <c r="G28" s="292"/>
-      <c r="H28" s="292"/>
-      <c r="I28" s="292"/>
+      <c r="C28" s="306"/>
+      <c r="D28" s="306"/>
+      <c r="E28" s="306"/>
+      <c r="F28" s="307"/>
+      <c r="G28" s="307"/>
+      <c r="H28" s="307"/>
+      <c r="I28" s="307"/>
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="2:10" ht="9" customHeight="1">
@@ -10492,19 +10047,19 @@
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" ht="18" customHeight="1" thickBot="1">
-      <c r="B31" s="293" t="s">
+      <c r="B31" s="308" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="294"/>
-      <c r="D31" s="294"/>
-      <c r="E31" s="295"/>
+      <c r="C31" s="309"/>
+      <c r="D31" s="309"/>
+      <c r="E31" s="310"/>
       <c r="F31" s="127"/>
-      <c r="G31" s="296" t="s">
+      <c r="G31" s="311" t="s">
         <v>70</v>
       </c>
-      <c r="H31" s="297"/>
-      <c r="I31" s="297"/>
-      <c r="J31" s="298"/>
+      <c r="H31" s="312"/>
+      <c r="I31" s="312"/>
+      <c r="J31" s="313"/>
     </row>
     <row r="32" spans="2:10" ht="13.9" customHeight="1">
       <c r="B32" s="63"/>
@@ -10514,89 +10069,89 @@
     <row r="33" spans="2:10" ht="12.6" customHeight="1">
       <c r="B33" s="4"/>
       <c r="E33" s="128"/>
-      <c r="F33" s="299"/>
-      <c r="G33" s="299"/>
-      <c r="H33" s="300"/>
-      <c r="I33" s="300"/>
+      <c r="F33" s="314"/>
+      <c r="G33" s="314"/>
+      <c r="H33" s="315"/>
+      <c r="I33" s="315"/>
       <c r="J33" s="5"/>
     </row>
     <row r="34" spans="2:10" ht="12.6" customHeight="1">
       <c r="B34" s="4"/>
       <c r="F34" s="123"/>
-      <c r="G34" s="301" t="s">
+      <c r="G34" s="316" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="302"/>
-      <c r="I34" s="302"/>
-      <c r="J34" s="303"/>
+      <c r="H34" s="317"/>
+      <c r="I34" s="317"/>
+      <c r="J34" s="318"/>
     </row>
     <row r="35" spans="2:10" ht="12.6" customHeight="1">
-      <c r="B35" s="281"/>
-      <c r="C35" s="282"/>
-      <c r="D35" s="282"/>
-      <c r="E35" s="282"/>
+      <c r="B35" s="296"/>
+      <c r="C35" s="297"/>
+      <c r="D35" s="297"/>
+      <c r="E35" s="297"/>
       <c r="F35" s="123"/>
-      <c r="G35" s="283" t="s">
+      <c r="G35" s="298" t="s">
         <v>40</v>
       </c>
-      <c r="H35" s="284"/>
-      <c r="I35" s="285" t="s">
+      <c r="H35" s="299"/>
+      <c r="I35" s="300" t="s">
         <v>41</v>
       </c>
-      <c r="J35" s="286"/>
+      <c r="J35" s="301"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1">
-      <c r="B36" s="265"/>
-      <c r="C36" s="266"/>
-      <c r="D36" s="266"/>
-      <c r="E36" s="266"/>
+      <c r="B36" s="280"/>
+      <c r="C36" s="281"/>
+      <c r="D36" s="281"/>
+      <c r="E36" s="281"/>
       <c r="F36" s="123"/>
-      <c r="G36" s="267" t="s">
+      <c r="G36" s="282" t="s">
         <v>71</v>
       </c>
-      <c r="H36" s="268"/>
-      <c r="I36" s="268"/>
-      <c r="J36" s="269"/>
+      <c r="H36" s="283"/>
+      <c r="I36" s="283"/>
+      <c r="J36" s="284"/>
     </row>
     <row r="37" spans="2:10" ht="10.15" customHeight="1" thickTop="1">
-      <c r="B37" s="270"/>
-      <c r="C37" s="271"/>
-      <c r="D37" s="271"/>
+      <c r="B37" s="285"/>
+      <c r="C37" s="286"/>
+      <c r="D37" s="286"/>
       <c r="E37" s="54"/>
-      <c r="F37" s="272"/>
-      <c r="G37" s="272"/>
-      <c r="H37" s="273"/>
-      <c r="I37" s="273"/>
+      <c r="F37" s="287"/>
+      <c r="G37" s="287"/>
+      <c r="H37" s="288"/>
+      <c r="I37" s="288"/>
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="2:10" ht="32.25" customHeight="1">
-      <c r="B38" s="274" t="s">
+      <c r="B38" s="289" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="275"/>
-      <c r="D38" s="275"/>
-      <c r="E38" s="276"/>
-      <c r="F38" s="276"/>
-      <c r="G38" s="276"/>
-      <c r="H38" s="276"/>
-      <c r="I38" s="276"/>
-      <c r="J38" s="277"/>
+      <c r="C38" s="290"/>
+      <c r="D38" s="290"/>
+      <c r="E38" s="291"/>
+      <c r="F38" s="291"/>
+      <c r="G38" s="291"/>
+      <c r="H38" s="291"/>
+      <c r="I38" s="291"/>
+      <c r="J38" s="292"/>
     </row>
     <row r="39" spans="2:10" ht="13.5" thickBot="1">
       <c r="B39" s="4"/>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="2:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B40" s="278" t="s">
+      <c r="B40" s="293" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="279"/>
-      <c r="D40" s="279"/>
-      <c r="E40" s="279"/>
-      <c r="F40" s="279"/>
-      <c r="G40" s="279"/>
-      <c r="H40" s="279"/>
-      <c r="I40" s="280"/>
+      <c r="C40" s="294"/>
+      <c r="D40" s="294"/>
+      <c r="E40" s="294"/>
+      <c r="F40" s="294"/>
+      <c r="G40" s="294"/>
+      <c r="H40" s="294"/>
+      <c r="I40" s="295"/>
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="2:10" ht="23.25" customHeight="1">
@@ -10610,8 +10165,8 @@
       <c r="B42" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="264"/>
-      <c r="D42" s="264"/>
+      <c r="C42" s="279"/>
+      <c r="D42" s="279"/>
       <c r="E42" s="13" t="s">
         <v>47</v>
       </c>
@@ -27736,6 +27291,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="ee5aff6a-8cf0-4458-8271-79e12eb440c2">
@@ -27758,7 +27322,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007B5F973EE7BF704CA893C4479403115B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="596c43eee58327b6c1b1d600265c86a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c9a3de0-7256-498b-bd58-38454e6e885f" xmlns:ns3="ee5aff6a-8cf0-4458-8271-79e12eb440c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e0a374b6e529ea9d86d827d90647bac" ns2:_="" ns3:_="">
     <xsd:import namespace="5c9a3de0-7256-498b-bd58-38454e6e885f"/>
@@ -27995,16 +27559,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{071FB459-7FD3-4170-A34B-9BDA43D5963B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAD9327-786D-428F-A038-9DCEFDE42568}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -28021,7 +27584,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DED1C6AB-442F-4580-B6A5-300A2E27DE13}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28038,12 +27601,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{071FB459-7FD3-4170-A34B-9BDA43D5963B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>